<commit_message>
Finished Unit 1 except additional examples on PCM1b
</commit_message>
<xml_diff>
--- a/Slide Names.xlsx
+++ b/Slide Names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiran\Desktop\ST 370 Redesign\ST-370\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F9381B0-7D3A-417C-B825-02D3C4F04B97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491CEEF3-AFF6-4047-B6B2-A81B40CE86E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{B8C04C7F-C8C3-490A-975E-25FA1614024B}"/>
   </bookViews>
@@ -30,14 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="218">
   <si>
     <t>Unit</t>
   </si>
   <si>
-    <t>Intro PCM</t>
-  </si>
-  <si>
     <t>Slide #</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
     <t>Recap of Ideas</t>
   </si>
   <si>
-    <t xml:space="preserve">Duplicate Slide; same as slide 3.23? </t>
-  </si>
-  <si>
     <t>McDonald's Example 1</t>
   </si>
   <si>
@@ -369,6 +363,327 @@
   </si>
   <si>
     <t>PCM1a</t>
+  </si>
+  <si>
+    <t>2 PCMb Part 1</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Distributions</t>
+  </si>
+  <si>
+    <t>Data - Pollution</t>
+  </si>
+  <si>
+    <t>Visualizing Distributions</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Finding Probabilities I</t>
+  </si>
+  <si>
+    <t>Finding Probabilities II</t>
+  </si>
+  <si>
+    <t>Helpful Probability Rules I</t>
+  </si>
+  <si>
+    <t>Helpful Probability Rules II</t>
+  </si>
+  <si>
+    <t>Helpful Probability Rules III</t>
+  </si>
+  <si>
+    <t>Visual - Additive Rule</t>
+  </si>
+  <si>
+    <t>Visual - Disjoint Probability</t>
+  </si>
+  <si>
+    <t>Helpful Probability Rules IV</t>
+  </si>
+  <si>
+    <t>Visual - Complement Rule</t>
+  </si>
+  <si>
+    <t>Summary - Probability Rules</t>
+  </si>
+  <si>
+    <t>Duplicate Slide; same as slide 3.23? No example content</t>
+  </si>
+  <si>
+    <t>Duplicate Slide; same as slide 3.23? No recap of ideas</t>
+  </si>
+  <si>
+    <t>Marketing Example 2 - Statistical Process</t>
+  </si>
+  <si>
+    <t>Check PCMa; slide incomplete</t>
+  </si>
+  <si>
+    <t>JUNTOS Example</t>
+  </si>
+  <si>
+    <t>PCM1b</t>
+  </si>
+  <si>
+    <t>Part 2: Take the Quiz?</t>
+  </si>
+  <si>
+    <t>Random Variables (RVs)</t>
+  </si>
+  <si>
+    <t>RVs and Inference</t>
+  </si>
+  <si>
+    <t>Discrete RVs Example</t>
+  </si>
+  <si>
+    <t>Discrete RVs - Proportion</t>
+  </si>
+  <si>
+    <t>Discrete RVs Distribution</t>
+  </si>
+  <si>
+    <t>Simulating  Distribution for Sample Proportion - Idea</t>
+  </si>
+  <si>
+    <t>Simulating  Distribution for Sample Proportion - Method</t>
+  </si>
+  <si>
+    <t>Simulating  Distribution for Sample Proportion - Results</t>
+  </si>
+  <si>
+    <t>Sampling Distribution Interpretation I</t>
+  </si>
+  <si>
+    <t>Sampling Distribution Interpretation II</t>
+  </si>
+  <si>
+    <t>PMFs</t>
+  </si>
+  <si>
+    <t>PMF Example - Poisson 1</t>
+  </si>
+  <si>
+    <t>PMF Example - Poisson 2</t>
+  </si>
+  <si>
+    <t>PMF Example - Poisson 3</t>
+  </si>
+  <si>
+    <t>PMF Recap</t>
+  </si>
+  <si>
+    <t>Continuous Random Variables</t>
+  </si>
+  <si>
+    <t>PDF Example - Exponential 1</t>
+  </si>
+  <si>
+    <t>PDF Example - Exponential 2</t>
+  </si>
+  <si>
+    <t>PDF Example - Exponential 3</t>
+  </si>
+  <si>
+    <t>PDF Example - Exponential 4</t>
+  </si>
+  <si>
+    <t>PDF Recap</t>
+  </si>
+  <si>
+    <t>CDFs 1</t>
+  </si>
+  <si>
+    <t>CDFS 2</t>
+  </si>
+  <si>
+    <t>Example 1 -  Client Contact (Poisson) I</t>
+  </si>
+  <si>
+    <t>Example 1 -  Client Contact (Poisson) II</t>
+  </si>
+  <si>
+    <t>Example 1 -  Client Contact (Poisson) III</t>
+  </si>
+  <si>
+    <t>Example 1 -  Client Contact (Poisson) IV</t>
+  </si>
+  <si>
+    <t>Example 1 -  Client Contact (Poisson) V</t>
+  </si>
+  <si>
+    <t>Example 2 - Call Centers (Poisson) I</t>
+  </si>
+  <si>
+    <t>Example 2 - Call Centers (Poisson) II</t>
+  </si>
+  <si>
+    <t>Example 2 - Call Centers (Poisson) III</t>
+  </si>
+  <si>
+    <t>3 PCMb Part 2</t>
+  </si>
+  <si>
+    <t>4 PCMb Review</t>
+  </si>
+  <si>
+    <t>Congrats!</t>
+  </si>
+  <si>
+    <t>PCM1c</t>
+  </si>
+  <si>
+    <t>Point Estimation</t>
+  </si>
+  <si>
+    <t>Common Point Estimators</t>
+  </si>
+  <si>
+    <t>Estimator vs Estimate</t>
+  </si>
+  <si>
+    <t>Estimator Example 1 - Vaccine I</t>
+  </si>
+  <si>
+    <t>Estimator Example 1 - Vaccine II</t>
+  </si>
+  <si>
+    <t>Estimator Example 1 - Vaccine III</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Example - Breast Cancer (Proportions Visual)</t>
+  </si>
+  <si>
+    <t>Estimator Example 2 - Parent Age at Birth (Mean) I</t>
+  </si>
+  <si>
+    <t>Estimator Example 2 - Parent Age at Birth (Mean) II</t>
+  </si>
+  <si>
+    <t>Estimator Example 2 - Parent Age at Birth (Mean) III</t>
+  </si>
+  <si>
+    <t>Limitations of Point Estimators (Proportions)</t>
+  </si>
+  <si>
+    <t>Limitations of Point Estimators (Means)</t>
+  </si>
+  <si>
+    <t>Standard Error (Means)</t>
+  </si>
+  <si>
+    <t>Standard Deviations</t>
+  </si>
+  <si>
+    <t>Margin of Error (Means)</t>
+  </si>
+  <si>
+    <t>Margin of Error (Proportions)</t>
+  </si>
+  <si>
+    <t>Example - Breast Cancer Tumor Size (Means)</t>
+  </si>
+  <si>
+    <t>Example - Breast Cancer (Proportions)</t>
+  </si>
+  <si>
+    <t>Example - Breast Cancer Tumor Size (Means Visual)</t>
+  </si>
+  <si>
+    <t>CI Example 2 - Pancreatic Cancer and Smoking (Proportions) III</t>
+  </si>
+  <si>
+    <t>CI Example 1 - Therapy (Proportions) I</t>
+  </si>
+  <si>
+    <t>CI Example 1 - Therapy (Proportions) II</t>
+  </si>
+  <si>
+    <t>CI Example 1 - Therapy (Proportions) III</t>
+  </si>
+  <si>
+    <t>CI Example 1 - Therapy (Proportions) IV</t>
+  </si>
+  <si>
+    <t>CI Example 1 - Therapy (Proportions) V</t>
+  </si>
+  <si>
+    <t>CI Example 2 - Pancreatic Cancer and Smoking (Proportions) I</t>
+  </si>
+  <si>
+    <t>CI Example 2 - Pancreatic Cancer and Smoking (Proportions) II</t>
+  </si>
+  <si>
+    <t>CI Example 2 - Pancreatic Cancer and Smoking (Proportions) IV</t>
+  </si>
+  <si>
+    <t>2 PCMc Part 1</t>
+  </si>
+  <si>
+    <t>3 PCMc Part 2</t>
+  </si>
+  <si>
+    <t>Confidence Interval: Idea</t>
+  </si>
+  <si>
+    <t>Confidence Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CI Example 3 - Breast Cancer (Calculation) </t>
+  </si>
+  <si>
+    <t>CI Interpretation I</t>
+  </si>
+  <si>
+    <t>CI Interpretation II</t>
+  </si>
+  <si>
+    <t>CI Interpretation III</t>
+  </si>
+  <si>
+    <t>CI Formula for Proportions I</t>
+  </si>
+  <si>
+    <t>CI Formula for Proportions II</t>
+  </si>
+  <si>
+    <t>CI Example 4: Allergies (Proportions) I</t>
+  </si>
+  <si>
+    <t>CI Example 4: Allergies (Proportions) II</t>
+  </si>
+  <si>
+    <t>Confidence Level Visual</t>
+  </si>
+  <si>
+    <t>CI Example 5: Einstein (Proportions) II</t>
+  </si>
+  <si>
+    <t>CI Example 5: Einstein (Proportions) I</t>
+  </si>
+  <si>
+    <t>CI Example 5: Einstein (Proportions) III</t>
+  </si>
+  <si>
+    <t>CI Example 6: Obama (Proportions) III</t>
+  </si>
+  <si>
+    <t>CI Example 6: Obama (Proportions) I</t>
+  </si>
+  <si>
+    <t>CI Example 6: Obama (Proportions) II</t>
+  </si>
+  <si>
+    <t>4 PCMc Review</t>
   </si>
 </sst>
 </file>
@@ -384,7 +699,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +709,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,13 +731,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -739,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895962D6-D221-4602-8123-4C7D8F01C46F}">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="B211" workbookViewId="0">
+      <selection activeCell="D251" sqref="D251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +1077,7 @@
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="66.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,1112 +1085,2570 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="D2">
         <v>1.1000000000000001</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="3"/>
       <c r="D3">
         <v>1.2</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3" t="s">
-        <v>39</v>
+      <c r="A4" s="4"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D4">
         <v>2.1</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="4"/>
       <c r="D5">
         <v>2.2000000000000002</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="4"/>
       <c r="D6">
         <v>2.2999999999999998</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="4"/>
       <c r="D7">
         <v>2.4</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="4"/>
       <c r="D8">
         <v>2.5</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="4"/>
       <c r="D9">
         <v>2.6</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="4"/>
       <c r="D10">
         <v>2.7</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="4"/>
       <c r="D11">
         <v>2.8</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="4"/>
       <c r="D12">
         <v>2.9</v>
       </c>
       <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="E13" t="s">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2">
-        <v>2.1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="3"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="4"/>
       <c r="D14">
         <v>2.11</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="3"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4"/>
       <c r="D15">
         <v>2.12</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="4"/>
       <c r="D16">
         <v>2.13</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="3"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="4"/>
       <c r="D17">
         <v>2.15</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4"/>
       <c r="D18">
         <v>2.16</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="4"/>
       <c r="D19">
         <v>2.17</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="3"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="4"/>
       <c r="D20">
         <v>2.1800000000000002</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="3"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="4"/>
       <c r="D21">
         <v>2.19</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="3"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="4"/>
       <c r="D22">
         <v>2.14</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="3"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="4"/>
       <c r="D23">
         <v>2.2599999999999998</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="3"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="4"/>
       <c r="D24">
         <v>2.27</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="1">
         <v>2.2000000000000002</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="3"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="4"/>
       <c r="D26">
         <v>2.21</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="3"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="4"/>
       <c r="D27">
         <v>2.2200000000000002</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="3"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="4"/>
       <c r="D28">
         <v>2.23</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="3"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="4"/>
       <c r="D29">
         <v>2.2400000000000002</v>
       </c>
       <c r="E29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="3"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="4"/>
       <c r="D30">
         <v>2.25</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="3" t="s">
-        <v>40</v>
+      <c r="A31" s="4"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="D31">
         <v>3.1</v>
       </c>
       <c r="E31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="3"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="4"/>
       <c r="D32">
         <v>3.2</v>
       </c>
       <c r="E32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="3"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="4"/>
       <c r="D33">
         <v>3.3</v>
       </c>
       <c r="E33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="3"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="4"/>
       <c r="D34">
         <v>3.4</v>
       </c>
       <c r="E34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="3"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="4"/>
       <c r="D35">
         <v>3.5</v>
       </c>
       <c r="E35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="3"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="4"/>
       <c r="D36">
         <v>3.6</v>
       </c>
       <c r="E36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="3"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="4"/>
       <c r="D37">
         <v>3.7</v>
       </c>
       <c r="E37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="3"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="4"/>
       <c r="D38">
         <v>3.8</v>
       </c>
       <c r="E38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="3"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="4"/>
       <c r="D39">
         <v>3.9</v>
       </c>
       <c r="E39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="1">
         <v>3.1</v>
       </c>
       <c r="E40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="3"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="4"/>
       <c r="D41">
         <v>3.11</v>
       </c>
       <c r="E41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="3"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="4"/>
       <c r="D42">
         <v>3.12</v>
       </c>
       <c r="E42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="3"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="4"/>
       <c r="D43">
         <v>3.13</v>
       </c>
       <c r="E43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="3"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="4"/>
       <c r="D44">
         <v>3.14</v>
       </c>
       <c r="E44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="3"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="4"/>
       <c r="D45">
         <v>3.15</v>
       </c>
       <c r="E45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="3"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="4"/>
       <c r="D46">
         <v>3.16</v>
       </c>
       <c r="E46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="3"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="4"/>
       <c r="D47">
         <v>3.17</v>
       </c>
       <c r="E47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="3"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="4"/>
       <c r="D48">
         <v>3.18</v>
       </c>
       <c r="E48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="3"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="4"/>
       <c r="D49">
         <v>3.19</v>
       </c>
       <c r="E49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="E50" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="2">
-        <v>3.2</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>60</v>
       </c>
-      <c r="F50" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="3"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="4"/>
       <c r="D51">
         <v>3.21</v>
       </c>
       <c r="E51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="3"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="4"/>
       <c r="D52">
         <v>3.22</v>
       </c>
       <c r="E52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="3"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="4"/>
       <c r="D53">
         <v>3.23</v>
       </c>
       <c r="E53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="3"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="4"/>
       <c r="D54">
         <v>3.24</v>
       </c>
       <c r="E54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="3"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="4"/>
       <c r="D55">
         <v>3.25</v>
       </c>
       <c r="E55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="3"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="4"/>
       <c r="D56">
         <v>3.26</v>
       </c>
       <c r="E56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="3"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="4"/>
       <c r="D57">
         <v>3.27</v>
       </c>
       <c r="E57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F57" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="3"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="4"/>
       <c r="D58">
         <v>3.28</v>
       </c>
       <c r="E58" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="3"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="4"/>
       <c r="D59">
         <v>3.29</v>
       </c>
       <c r="E59" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="1">
         <v>3.3</v>
       </c>
       <c r="E60" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="3"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="4"/>
       <c r="D61">
         <v>3.31</v>
       </c>
       <c r="E61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="3"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="4"/>
       <c r="D62">
         <v>3.39</v>
       </c>
       <c r="E62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="1">
         <v>3.4</v>
       </c>
       <c r="E63" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="3"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="4"/>
       <c r="D64">
         <v>3.32</v>
       </c>
       <c r="E64" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F64" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="3"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="4"/>
       <c r="D65">
         <v>3.33</v>
       </c>
       <c r="E65" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="3"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="4"/>
       <c r="D66">
         <v>3.34</v>
       </c>
       <c r="E66" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="3"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="4"/>
       <c r="D67">
         <v>3.35</v>
       </c>
       <c r="E67" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="3"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="4"/>
       <c r="D68">
         <v>3.36</v>
       </c>
       <c r="E68" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="3"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="4"/>
       <c r="D69">
         <v>3.37</v>
       </c>
       <c r="E69" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="3"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="4"/>
       <c r="D70">
         <v>3.38</v>
       </c>
       <c r="E70" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="3" t="s">
-        <v>83</v>
+      <c r="A71" s="4"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="D71">
         <v>4.0999999999999996</v>
       </c>
       <c r="E71" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="3"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="4"/>
       <c r="D72">
         <v>4.2</v>
       </c>
       <c r="E72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="3"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="4"/>
       <c r="D73">
         <v>4.3</v>
       </c>
       <c r="E73" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="3"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="4"/>
       <c r="D74">
         <v>4.4000000000000004</v>
       </c>
       <c r="E74" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="3"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="4"/>
       <c r="D75">
         <v>4.5</v>
       </c>
       <c r="E75" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="3"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="4"/>
       <c r="D76">
         <v>4.5999999999999996</v>
       </c>
       <c r="E76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="3"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="4"/>
       <c r="D77">
         <v>4.7</v>
       </c>
       <c r="E77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="3"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="4"/>
       <c r="D78">
         <v>4.8</v>
       </c>
       <c r="E78" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="3"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="4"/>
       <c r="D79">
         <v>4.9000000000000004</v>
       </c>
       <c r="E79" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E80" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="3"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="2">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E80" t="s">
-        <v>93</v>
-      </c>
-    </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="3"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="3"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="4"/>
       <c r="D81">
         <v>4.1100000000000003</v>
       </c>
       <c r="E81" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="3"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="3"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="4"/>
       <c r="D82">
         <v>4.12</v>
       </c>
       <c r="E82" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="3"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="4"/>
       <c r="D83">
         <v>4.13</v>
       </c>
       <c r="E83" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="3"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="3"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="4"/>
       <c r="D84">
         <v>4.1399999999999997</v>
       </c>
       <c r="E84" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="3"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="3"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="4"/>
       <c r="D85">
         <v>4.1500000000000004</v>
       </c>
       <c r="E85" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="3"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="4"/>
       <c r="D86">
         <v>4.16</v>
       </c>
       <c r="E86" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
-      <c r="B87" s="5"/>
-      <c r="C87" s="3"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="4"/>
       <c r="D87">
         <v>4.17</v>
       </c>
       <c r="E87" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="3"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="4"/>
       <c r="D88">
         <v>4.2300000000000004</v>
       </c>
       <c r="E88" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="3"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="3"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="4"/>
       <c r="D89">
         <v>4.24</v>
       </c>
       <c r="E89" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="3"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="3"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="4"/>
       <c r="D90">
         <v>4.18</v>
       </c>
       <c r="E90" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F90" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="3"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="3"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="4"/>
       <c r="D91">
         <v>4.1900000000000004</v>
       </c>
       <c r="E91" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="3"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="2">
+      <c r="A92" s="4"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="1">
         <v>4.2</v>
       </c>
       <c r="E92" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="3"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="4"/>
       <c r="D93">
         <v>4.21</v>
       </c>
       <c r="E93" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="3"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="3"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="4"/>
       <c r="D94">
         <v>4.22</v>
       </c>
       <c r="E94" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="5"/>
-      <c r="C95" s="4" t="s">
-        <v>108</v>
+      <c r="B95" s="7"/>
+      <c r="C95" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="D95">
         <v>5.0999999999999996</v>
       </c>
       <c r="E95" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B96" s="5"/>
-      <c r="C96" s="4"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="6"/>
       <c r="D96">
         <v>5.2</v>
       </c>
       <c r="E96" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
-        <v>1</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D97">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="5"/>
+      <c r="C98" s="3"/>
+      <c r="D98">
+        <v>1.2</v>
+      </c>
+      <c r="E98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="5"/>
+      <c r="C99" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D99">
+        <v>2.1</v>
+      </c>
+      <c r="E99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="5"/>
+      <c r="C100" s="4"/>
+      <c r="D100">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E100" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="5"/>
+      <c r="C101" s="4"/>
+      <c r="D101">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="5"/>
+      <c r="C102" s="4"/>
+      <c r="D102">
+        <v>2.4</v>
+      </c>
+      <c r="E102" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="5"/>
+      <c r="C103" s="4"/>
+      <c r="D103">
+        <v>2.5</v>
+      </c>
+      <c r="E103" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="5"/>
+      <c r="C104" s="4"/>
+      <c r="D104">
+        <v>2.6</v>
+      </c>
+      <c r="E104" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="5"/>
+      <c r="C105" s="4"/>
+      <c r="D105">
+        <v>2.7</v>
+      </c>
+      <c r="E105" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106" s="5"/>
+      <c r="C106" s="4"/>
+      <c r="D106">
+        <v>2.8</v>
+      </c>
+      <c r="E106" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="5"/>
+      <c r="C107" s="4"/>
+      <c r="D107">
+        <v>2.9</v>
+      </c>
+      <c r="E107" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="5"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="E108" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109" s="5"/>
+      <c r="C109" s="4"/>
+      <c r="D109">
+        <v>2.11</v>
+      </c>
+      <c r="E109" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110" s="5"/>
+      <c r="C110" s="4"/>
+      <c r="D110">
+        <v>2.12</v>
+      </c>
+      <c r="E110" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="5"/>
+      <c r="C111" s="4"/>
+      <c r="D111">
+        <v>2.13</v>
+      </c>
+      <c r="E111" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B112" s="5"/>
+      <c r="C112" s="4"/>
+      <c r="D112">
+        <v>2.14</v>
+      </c>
+      <c r="E112" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B113" s="5"/>
+      <c r="C113" s="4"/>
+      <c r="D113">
+        <v>2.15</v>
+      </c>
+      <c r="E113" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B114" s="5"/>
+      <c r="C114" s="4"/>
+      <c r="D114">
+        <v>2.16</v>
+      </c>
+      <c r="E114" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B115" s="5"/>
+      <c r="C115" s="4"/>
+      <c r="D115">
+        <v>2.17</v>
+      </c>
+      <c r="E115" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B116" s="5"/>
+      <c r="C116" s="4"/>
+      <c r="D116">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E116" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B117" s="5"/>
+      <c r="C117" s="4"/>
+      <c r="D117">
+        <v>2.19</v>
+      </c>
+      <c r="E117" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B118" s="5"/>
+      <c r="C118" s="4"/>
+      <c r="D118">
+        <v>2.21</v>
+      </c>
+      <c r="E118" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B119" s="5"/>
+      <c r="C119" s="4"/>
+      <c r="D119">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="E119" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B120" s="5"/>
+      <c r="C120" s="4"/>
+      <c r="D120">
+        <v>2.23</v>
+      </c>
+      <c r="E120" t="s">
+        <v>23</v>
+      </c>
+      <c r="F120" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B121" s="5"/>
+      <c r="C121" s="4"/>
+      <c r="D121">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E121" t="s">
+        <v>129</v>
+      </c>
+      <c r="F121" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B122" s="5"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E122" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B123" s="5"/>
+      <c r="C123" s="4"/>
+      <c r="D123">
+        <v>2.29</v>
+      </c>
+      <c r="E123" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B124" s="5"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E124" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B125" s="5"/>
+      <c r="C125" s="4"/>
+      <c r="D125">
+        <v>2.25</v>
+      </c>
+      <c r="E125" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B126" s="5"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="1">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="E126" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B127" s="5"/>
+      <c r="C127" s="4"/>
+      <c r="D127">
+        <v>2.27</v>
+      </c>
+      <c r="E127" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B128" s="5"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="1">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E128" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129" s="5"/>
+      <c r="C129" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D129">
+        <v>3.1</v>
+      </c>
+      <c r="E129" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B130" s="5"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="E130" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131" s="5"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E131" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132" s="5"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="E132" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B133" s="5"/>
+      <c r="C133" s="4"/>
+      <c r="D133" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="E133" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B134" s="5"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="E134" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B135" s="5"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="E135" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B136" s="5"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="E136" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B137" s="5"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="E137" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B138" s="5"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="E138" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B139" s="5"/>
+      <c r="C139" s="4"/>
+      <c r="D139" s="2">
+        <v>3.11</v>
+      </c>
+      <c r="E139" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B140" s="5"/>
+      <c r="C140" s="4"/>
+      <c r="D140" s="2">
+        <v>3.12</v>
+      </c>
+      <c r="E140" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B141" s="5"/>
+      <c r="C141" s="4"/>
+      <c r="D141" s="2">
+        <v>3.13</v>
+      </c>
+      <c r="E141" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B142" s="5"/>
+      <c r="C142" s="4"/>
+      <c r="D142" s="2">
+        <v>3.14</v>
+      </c>
+      <c r="E142" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B143" s="5"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="2">
+        <v>3.15</v>
+      </c>
+      <c r="E143" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B144" s="5"/>
+      <c r="C144" s="4"/>
+      <c r="D144" s="2">
+        <v>3.16</v>
+      </c>
+      <c r="E144" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B145" s="5"/>
+      <c r="C145" s="4"/>
+      <c r="D145" s="2">
+        <v>3.17</v>
+      </c>
+      <c r="E145" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B146" s="5"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="2">
+        <v>3.18</v>
+      </c>
+      <c r="E146" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B147" s="5"/>
+      <c r="C147" s="4"/>
+      <c r="D147" s="2">
+        <v>3.19</v>
+      </c>
+      <c r="E147" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="5"/>
+      <c r="C148" s="4"/>
+      <c r="D148" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="E148" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B149" s="5"/>
+      <c r="C149" s="4"/>
+      <c r="D149" s="2">
+        <v>3.21</v>
+      </c>
+      <c r="E149" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B150" s="5"/>
+      <c r="C150" s="4"/>
+      <c r="D150" s="2">
+        <v>3.22</v>
+      </c>
+      <c r="E150" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B151" s="5"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="2">
+        <v>3.23</v>
+      </c>
+      <c r="E151" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B152" s="5"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="2">
+        <v>3.24</v>
+      </c>
+      <c r="E152" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B153" s="5"/>
+      <c r="C153" s="4"/>
+      <c r="D153" s="2">
+        <v>3.25</v>
+      </c>
+      <c r="E153" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B154" s="5"/>
+      <c r="C154" s="4"/>
+      <c r="D154" s="2">
+        <v>3.26</v>
+      </c>
+      <c r="E154" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B155" s="5"/>
+      <c r="C155" s="4"/>
+      <c r="D155" s="2">
+        <v>3.27</v>
+      </c>
+      <c r="E155" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B156" s="5"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="2">
+        <v>3.28</v>
+      </c>
+      <c r="E156" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B157" s="5"/>
+      <c r="C157" s="4"/>
+      <c r="D157" s="2">
+        <v>3.29</v>
+      </c>
+      <c r="E157" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="158" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B158" s="5"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="E158" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B159" s="5"/>
+      <c r="C159" s="4"/>
+      <c r="D159" s="2">
+        <v>3.31</v>
+      </c>
+      <c r="E159" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B160" s="5"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="2">
+        <v>3.32</v>
+      </c>
+      <c r="E160" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B161" s="5"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="2">
+        <v>3.33</v>
+      </c>
+      <c r="E161" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B162" s="5"/>
+      <c r="C162" s="4"/>
+      <c r="D162" s="2">
+        <v>3.34</v>
+      </c>
+      <c r="E162" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B163" s="5"/>
+      <c r="C163" s="4"/>
+      <c r="D163" s="2">
+        <v>3.35</v>
+      </c>
+      <c r="E163" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B164" s="5"/>
+      <c r="C164" s="4"/>
+      <c r="D164" s="2">
+        <v>3.42</v>
+      </c>
+      <c r="E164" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B165" s="5"/>
+      <c r="C165" s="4"/>
+      <c r="D165" s="2">
+        <v>3.43</v>
+      </c>
+      <c r="E165" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B166" s="5"/>
+      <c r="C166" s="4"/>
+      <c r="D166" s="2">
+        <v>3.36</v>
+      </c>
+      <c r="E166" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B167" s="5"/>
+      <c r="C167" s="4"/>
+      <c r="D167" s="2">
+        <v>3.37</v>
+      </c>
+      <c r="E167" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B168" s="5"/>
+      <c r="C168" s="4"/>
+      <c r="D168" s="2">
+        <v>3.38</v>
+      </c>
+      <c r="E168" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B169" s="5"/>
+      <c r="C169" s="4"/>
+      <c r="D169" s="2">
+        <v>3.39</v>
+      </c>
+      <c r="E169" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B170" s="5"/>
+      <c r="C170" s="4"/>
+      <c r="D170" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="E170" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="171" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B171" s="5"/>
+      <c r="C171" s="4"/>
+      <c r="D171">
+        <v>3.41</v>
+      </c>
+      <c r="E171" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="172" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B172" s="5"/>
+      <c r="C172" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D172">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E172" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="173" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B173" s="5"/>
+      <c r="C173" s="4"/>
+      <c r="D173">
+        <v>4.2</v>
+      </c>
+      <c r="E173" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="174" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B174" s="5"/>
+      <c r="C174" s="4"/>
+      <c r="D174">
+        <v>4.3</v>
+      </c>
+      <c r="E174" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="175" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
+        <v>168</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D175">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E175" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C176" s="3"/>
+      <c r="D176">
+        <v>1.2</v>
+      </c>
+      <c r="E176" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C177" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D177">
+        <v>2.1</v>
+      </c>
+      <c r="E177" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C178" s="4"/>
+      <c r="D178">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E178" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C179" s="4"/>
+      <c r="D179">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E179" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="180" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C180" s="4"/>
+      <c r="D180">
+        <v>2.4</v>
+      </c>
+      <c r="E180" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="181" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C181" s="4"/>
+      <c r="D181">
+        <v>2.5</v>
+      </c>
+      <c r="E181" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="182" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C182" s="4"/>
+      <c r="D182">
+        <v>2.6</v>
+      </c>
+      <c r="E182" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="183" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C183" s="4"/>
+      <c r="D183">
+        <v>2.7</v>
+      </c>
+      <c r="E183" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="184" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C184" s="4"/>
+      <c r="D184">
+        <v>2.8</v>
+      </c>
+      <c r="E184" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="185" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C185" s="4"/>
+      <c r="D185">
+        <v>2.9</v>
+      </c>
+      <c r="E185" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="186" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C186" s="4"/>
+      <c r="D186" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="E186" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="187" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C187" s="4"/>
+      <c r="D187">
+        <v>2.11</v>
+      </c>
+      <c r="E187" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="188" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C188" s="4"/>
+      <c r="D188">
+        <v>2.12</v>
+      </c>
+      <c r="E188" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="189" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C189" s="4"/>
+      <c r="D189">
+        <v>2.13</v>
+      </c>
+      <c r="E189" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="190" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C190" s="4"/>
+      <c r="D190">
+        <v>2.14</v>
+      </c>
+      <c r="E190" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="191" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C191" s="4"/>
+      <c r="D191">
+        <v>2.15</v>
+      </c>
+      <c r="E191" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="192" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C192" s="4"/>
+      <c r="D192">
+        <v>2.16</v>
+      </c>
+      <c r="E192" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="193" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C193" s="4"/>
+      <c r="D193">
+        <v>2.17</v>
+      </c>
+      <c r="E193" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="194" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C194" s="4"/>
+      <c r="D194">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E194" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="195" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C195" s="4"/>
+      <c r="D195">
+        <v>2.19</v>
+      </c>
+      <c r="E195" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="196" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C196" s="4"/>
+      <c r="D196" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E196" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="197" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C197" s="4"/>
+      <c r="D197">
+        <v>2.21</v>
+      </c>
+      <c r="E197" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="198" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C198" s="4"/>
+      <c r="D198">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="E198" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="199" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C199" s="4"/>
+      <c r="D199">
+        <v>2.23</v>
+      </c>
+      <c r="E199" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="200" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C200" s="4"/>
+      <c r="D200">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E200" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="201" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C201" s="4"/>
+      <c r="D201">
+        <v>2.25</v>
+      </c>
+      <c r="E201" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="202" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C202" s="4"/>
+      <c r="D202">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="E202" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="203" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C203" s="4"/>
+      <c r="D203">
+        <v>2.27</v>
+      </c>
+      <c r="E203" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="204" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C204" s="4"/>
+      <c r="D204">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E204" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="205" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C205" s="4"/>
+      <c r="D205">
+        <v>2.29</v>
+      </c>
+      <c r="E205" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="206" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C206" s="4"/>
+      <c r="D206" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E206" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="207" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C207" s="4"/>
+      <c r="D207">
+        <v>2.31</v>
+      </c>
+      <c r="E207" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="208" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C208" s="4"/>
+      <c r="D208">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="E208" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="209" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C209" s="4"/>
+      <c r="D209">
+        <v>2.33</v>
+      </c>
+      <c r="E209" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="210" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C210" s="4"/>
+      <c r="D210">
+        <v>2.34</v>
+      </c>
+      <c r="E210" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="211" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C211" s="4"/>
+      <c r="D211">
+        <v>2.35</v>
+      </c>
+      <c r="E211" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="212" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C212" s="4"/>
+      <c r="D212">
+        <v>2.36</v>
+      </c>
+      <c r="E212" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="213" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C213" s="4"/>
+      <c r="D213">
+        <v>2.37</v>
+      </c>
+      <c r="E213" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="214" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C214" s="4"/>
+      <c r="D214">
+        <v>2.38</v>
+      </c>
+      <c r="E214" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="215" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C215" s="4"/>
+      <c r="D215">
+        <v>2.39</v>
+      </c>
+      <c r="E215" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="216" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C216" s="4"/>
+      <c r="D216" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="E216" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="217" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C217" s="4"/>
+      <c r="D217">
+        <v>2.41</v>
+      </c>
+      <c r="E217" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="218" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C218" s="4"/>
+      <c r="D218">
+        <v>2.42</v>
+      </c>
+      <c r="E218" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="219" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C219" t="s">
+        <v>199</v>
+      </c>
+      <c r="D219">
+        <v>3.1</v>
+      </c>
+      <c r="E219" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="220" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D220">
+        <v>3.2</v>
+      </c>
+      <c r="E220" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="221" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D221">
+        <v>3.3</v>
+      </c>
+      <c r="E221" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="222" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D222">
+        <v>3.4</v>
+      </c>
+      <c r="E222" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="223" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D223">
+        <v>3.5</v>
+      </c>
+      <c r="E223" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="224" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D224">
+        <v>3.6</v>
+      </c>
+      <c r="E224" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="225" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D225">
+        <v>3.7</v>
+      </c>
+      <c r="E225" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="226" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D226">
+        <v>3.8</v>
+      </c>
+      <c r="E226" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="227" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D227">
+        <v>3.9</v>
+      </c>
+      <c r="E227" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="228" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D228" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="E228" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="229" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D229">
+        <v>3.11</v>
+      </c>
+      <c r="E229" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="230" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D230">
+        <v>3.12</v>
+      </c>
+      <c r="E230" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="231" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D231">
+        <v>3.13</v>
+      </c>
+      <c r="E231" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="232" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D232">
+        <v>3.14</v>
+      </c>
+      <c r="E232" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="233" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D233">
+        <v>3.15</v>
+      </c>
+      <c r="E233" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="234" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D234">
+        <v>3.16</v>
+      </c>
+      <c r="E234" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="235" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D235">
+        <v>3.17</v>
+      </c>
+      <c r="E235" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="236" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D236">
+        <v>3.18</v>
+      </c>
+      <c r="E236" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="237" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D237">
+        <v>3.19</v>
+      </c>
+      <c r="E237" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="238" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D238" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="E238" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="239" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D239">
+        <v>3.21</v>
+      </c>
+      <c r="E239" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="240" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D240">
+        <v>3.28</v>
+      </c>
+      <c r="E240" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="241" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D241" s="1">
+        <v>3.29</v>
+      </c>
+      <c r="E241" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="242" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D242">
+        <v>3.22</v>
+      </c>
+      <c r="E242" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="243" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D243">
+        <v>3.23</v>
+      </c>
+      <c r="E243" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="244" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D244">
+        <v>3.24</v>
+      </c>
+      <c r="E244" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="245" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D245">
+        <v>3.25</v>
+      </c>
+      <c r="E245" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="246" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D246">
+        <v>3.26</v>
+      </c>
+      <c r="E246" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="247" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D247">
+        <v>3.27</v>
+      </c>
+      <c r="E247" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="248" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C248" t="s">
+        <v>217</v>
+      </c>
+      <c r="D248">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E248" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="249" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D249">
+        <v>4.2</v>
+      </c>
+      <c r="E249" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="250" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D250">
+        <v>4.3</v>
+      </c>
+      <c r="E250" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
+    <mergeCell ref="C177:C218"/>
+    <mergeCell ref="B97:B174"/>
     <mergeCell ref="C31:C70"/>
     <mergeCell ref="C71:C94"/>
     <mergeCell ref="A2:A94"/>
@@ -1873,6 +3656,11 @@
     <mergeCell ref="B2:B96"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C30"/>
+    <mergeCell ref="C175:C176"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C99:C128"/>
+    <mergeCell ref="C129:C171"/>
+    <mergeCell ref="C172:C174"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated typset for examples on PCM1b
</commit_message>
<xml_diff>
--- a/Slide Names.xlsx
+++ b/Slide Names.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiran\Desktop\ST 370 Redesign\ST-370\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC75395-1925-45A7-BEE8-87AFE8DF0784}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{29EF78C6-8A78-425B-B446-288461183432}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{B8C04C7F-C8C3-490A-975E-25FA1614024B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{B8C04C7F-C8C3-490A-975E-25FA1614024B}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit 1" sheetId="1" r:id="rId1"/>
     <sheet name="Unit 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Unit 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="320">
   <si>
     <t>Unit</t>
   </si>
@@ -805,6 +807,192 @@
   </si>
   <si>
     <t>4 PCMa Review</t>
+  </si>
+  <si>
+    <t>PCM3a</t>
+  </si>
+  <si>
+    <t>Intro PCM</t>
+  </si>
+  <si>
+    <t>Hypothesis Test for Two Proportions</t>
+  </si>
+  <si>
+    <t>Recap: Population vs Sample</t>
+  </si>
+  <si>
+    <t>Sampling and Experiments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Sampling and Experiments 2</t>
+  </si>
+  <si>
+    <t>Sampling and Experiments 3</t>
+  </si>
+  <si>
+    <t>Sampling and Experiments 4</t>
+  </si>
+  <si>
+    <t>Experiments</t>
+  </si>
+  <si>
+    <t>Experiments 2</t>
+  </si>
+  <si>
+    <t>Experiments 3</t>
+  </si>
+  <si>
+    <t>Experiments 4</t>
+  </si>
+  <si>
+    <t>Experiments 5</t>
+  </si>
+  <si>
+    <t>Experiments 6</t>
+  </si>
+  <si>
+    <t>Experiments 7</t>
+  </si>
+  <si>
+    <t>Experiments 8</t>
+  </si>
+  <si>
+    <t>Example:  Experiment - Vitamin Supplements</t>
+  </si>
+  <si>
+    <t>Example:  Experiment - Vitamin Supplements 2</t>
+  </si>
+  <si>
+    <t>Example:  Experiment - Surface Roghness</t>
+  </si>
+  <si>
+    <t>Example:  Experiment - Surface Roghness 2</t>
+  </si>
+  <si>
+    <t>Example:  Experiment - Surface Roghness 3</t>
+  </si>
+  <si>
+    <t>Example:  Experiment - Tensile Strength</t>
+  </si>
+  <si>
+    <t>Example:  Experiment - Tensile Strength 2</t>
+  </si>
+  <si>
+    <t>Sources of Variability</t>
+  </si>
+  <si>
+    <t>Motivational Example: Weight Gain Experiment</t>
+  </si>
+  <si>
+    <t>Sources of Variability 2</t>
+  </si>
+  <si>
+    <t>Experimantal Error</t>
+  </si>
+  <si>
+    <t>Recognizing Sources of Variability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recognizing Sources of Variability - Variables Accounted </t>
+  </si>
+  <si>
+    <t>Recognizing Sources of Variability - Experimental Error</t>
+  </si>
+  <si>
+    <t>Recognizing Sources of Variability - Experimental Error 2</t>
+  </si>
+  <si>
+    <t>DOE</t>
+  </si>
+  <si>
+    <t>Reducing Experimental Error</t>
+  </si>
+  <si>
+    <t>Reducing Experimental Error 2</t>
+  </si>
+  <si>
+    <t>Reducing Experimental Error 3</t>
+  </si>
+  <si>
+    <t>Reducing Experimental Error 4</t>
+  </si>
+  <si>
+    <t>Pillars of DOE</t>
+  </si>
+  <si>
+    <t>Completely Randomized Design (CRD)</t>
+  </si>
+  <si>
+    <t>CRD vs SRS</t>
+  </si>
+  <si>
+    <t>Replication</t>
+  </si>
+  <si>
+    <t>Replication 2</t>
+  </si>
+  <si>
+    <t>Example - Ionizing Radiation</t>
+  </si>
+  <si>
+    <t>Example - Ionizing Radiation 2</t>
+  </si>
+  <si>
+    <t>Example - Ionizing Radiation 3</t>
+  </si>
+  <si>
+    <t>Example - Ionizing Radiation 4</t>
+  </si>
+  <si>
+    <t>Example - Crop Yield</t>
+  </si>
+  <si>
+    <t>Example - Crop Yield 2</t>
+  </si>
+  <si>
+    <t>Example - Crop Yield 3</t>
+  </si>
+  <si>
+    <t>Example - Insomnia</t>
+  </si>
+  <si>
+    <t>Example - Insomnia 2</t>
+  </si>
+  <si>
+    <t>PCM3b</t>
+  </si>
+  <si>
+    <t>Inference for Poportions (Two Sample)</t>
+  </si>
+  <si>
+    <t>Inference for Poportions (Two Sample) - In Context</t>
+  </si>
+  <si>
+    <t>Binomial Distribution -  PMF</t>
+  </si>
+  <si>
+    <t>Binomial Distribution -  Expectation</t>
+  </si>
+  <si>
+    <t>Binomial Distribution - Variance</t>
+  </si>
+  <si>
+    <t>Binomial Distribution - CLT</t>
+  </si>
+  <si>
+    <t>Sample Proprtion -  Expected Value</t>
+  </si>
+  <si>
+    <t>Sample Proprtion -  Variance</t>
+  </si>
+  <si>
+    <t>Sample Proprtion - CLT</t>
+  </si>
+  <si>
+    <t>CLT -  Idea</t>
   </si>
 </sst>
 </file>
@@ -820,7 +1008,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -839,6 +1027,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -852,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -860,9 +1054,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -873,6 +1064,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1190,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895962D6-D221-4602-8123-4C7D8F01C46F}">
   <dimension ref="A1:F254"/>
   <sheetViews>
-    <sheetView topLeftCell="B169" workbookViewId="0">
-      <selection activeCell="E176" sqref="E176:E178"/>
+    <sheetView topLeftCell="B246" workbookViewId="0">
+      <selection activeCell="D252" sqref="D252:E254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,10 +1425,10 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D2">
@@ -1243,8 +1440,8 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3">
         <v>1.2</v>
       </c>
@@ -1254,7 +1451,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
         <v>38</v>
       </c>
@@ -1267,7 +1464,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="7"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5">
         <v>2.2000000000000002</v>
@@ -1278,7 +1475,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="7"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6">
         <v>2.2999999999999998</v>
@@ -1289,7 +1486,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="7"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7">
         <v>2.4</v>
@@ -1300,7 +1497,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="7"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8">
         <v>2.5</v>
@@ -1311,7 +1508,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="7"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9">
         <v>2.6</v>
@@ -1322,7 +1519,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="7"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10">
         <v>2.7</v>
@@ -1336,7 +1533,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="7"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11">
         <v>2.8</v>
@@ -1347,7 +1544,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="7"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12">
         <v>2.9</v>
@@ -1361,7 +1558,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="7"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="1">
         <v>2.1</v>
@@ -1372,7 +1569,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="4"/>
       <c r="D14">
         <v>2.11</v>
@@ -1383,7 +1580,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="7"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="4"/>
       <c r="D15">
         <v>2.12</v>
@@ -1397,7 +1594,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="7"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="4"/>
       <c r="D16">
         <v>2.13</v>
@@ -1408,7 +1605,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="7"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="4"/>
       <c r="D17">
         <v>2.15</v>
@@ -1422,7 +1619,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="4"/>
       <c r="D18">
         <v>2.16</v>
@@ -1433,7 +1630,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="4"/>
       <c r="D19">
         <v>2.17</v>
@@ -1444,7 +1641,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="4"/>
       <c r="D20">
         <v>2.1800000000000002</v>
@@ -1455,7 +1652,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="4"/>
       <c r="D21">
         <v>2.19</v>
@@ -1466,7 +1663,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="4"/>
       <c r="D22">
         <v>2.14</v>
@@ -1477,7 +1674,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="7"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="4"/>
       <c r="D23">
         <v>2.2599999999999998</v>
@@ -1488,7 +1685,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="4"/>
       <c r="D24">
         <v>2.27</v>
@@ -1499,7 +1696,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="4"/>
       <c r="D25" s="1">
         <v>2.2000000000000002</v>
@@ -1513,7 +1710,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="7"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="4"/>
       <c r="D26">
         <v>2.21</v>
@@ -1524,7 +1721,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="4"/>
       <c r="D27">
         <v>2.2200000000000002</v>
@@ -1535,7 +1732,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="7"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="4"/>
       <c r="D28">
         <v>2.23</v>
@@ -1546,7 +1743,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="7"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="4"/>
       <c r="D29">
         <v>2.2400000000000002</v>
@@ -1557,7 +1754,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="7"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="4"/>
       <c r="D30">
         <v>2.25</v>
@@ -1568,7 +1765,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="7"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="4" t="s">
         <v>39</v>
       </c>
@@ -1581,7 +1778,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="7"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="4"/>
       <c r="D32">
         <v>3.2</v>
@@ -1592,7 +1789,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="7"/>
+      <c r="B33" s="6"/>
       <c r="C33" s="4"/>
       <c r="D33">
         <v>3.3</v>
@@ -1603,7 +1800,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="7"/>
+      <c r="B34" s="6"/>
       <c r="C34" s="4"/>
       <c r="D34">
         <v>3.4</v>
@@ -1614,7 +1811,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="7"/>
+      <c r="B35" s="6"/>
       <c r="C35" s="4"/>
       <c r="D35">
         <v>3.5</v>
@@ -1625,7 +1822,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="7"/>
+      <c r="B36" s="6"/>
       <c r="C36" s="4"/>
       <c r="D36">
         <v>3.6</v>
@@ -1636,7 +1833,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="7"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="4"/>
       <c r="D37">
         <v>3.7</v>
@@ -1647,7 +1844,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="7"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="4"/>
       <c r="D38">
         <v>3.8</v>
@@ -1658,7 +1855,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="7"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="4"/>
       <c r="D39">
         <v>3.9</v>
@@ -1669,7 +1866,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="7"/>
+      <c r="B40" s="6"/>
       <c r="C40" s="4"/>
       <c r="D40" s="1">
         <v>3.1</v>
@@ -1680,7 +1877,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="7"/>
+      <c r="B41" s="6"/>
       <c r="C41" s="4"/>
       <c r="D41">
         <v>3.11</v>
@@ -1691,7 +1888,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="7"/>
+      <c r="B42" s="6"/>
       <c r="C42" s="4"/>
       <c r="D42">
         <v>3.12</v>
@@ -1702,7 +1899,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="7"/>
+      <c r="B43" s="6"/>
       <c r="C43" s="4"/>
       <c r="D43">
         <v>3.13</v>
@@ -1713,7 +1910,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="7"/>
+      <c r="B44" s="6"/>
       <c r="C44" s="4"/>
       <c r="D44">
         <v>3.14</v>
@@ -1724,7 +1921,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="7"/>
+      <c r="B45" s="6"/>
       <c r="C45" s="4"/>
       <c r="D45">
         <v>3.15</v>
@@ -1735,7 +1932,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="7"/>
+      <c r="B46" s="6"/>
       <c r="C46" s="4"/>
       <c r="D46">
         <v>3.16</v>
@@ -1746,7 +1943,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
-      <c r="B47" s="7"/>
+      <c r="B47" s="6"/>
       <c r="C47" s="4"/>
       <c r="D47">
         <v>3.17</v>
@@ -1757,7 +1954,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
-      <c r="B48" s="7"/>
+      <c r="B48" s="6"/>
       <c r="C48" s="4"/>
       <c r="D48">
         <v>3.18</v>
@@ -1768,7 +1965,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="7"/>
+      <c r="B49" s="6"/>
       <c r="C49" s="4"/>
       <c r="D49">
         <v>3.19</v>
@@ -1779,7 +1976,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="7"/>
+      <c r="B50" s="6"/>
       <c r="C50" s="4"/>
       <c r="D50" s="1">
         <v>3.2</v>
@@ -1793,7 +1990,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
-      <c r="B51" s="7"/>
+      <c r="B51" s="6"/>
       <c r="C51" s="4"/>
       <c r="D51">
         <v>3.21</v>
@@ -1804,7 +2001,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
-      <c r="B52" s="7"/>
+      <c r="B52" s="6"/>
       <c r="C52" s="4"/>
       <c r="D52">
         <v>3.22</v>
@@ -1815,7 +2012,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
-      <c r="B53" s="7"/>
+      <c r="B53" s="6"/>
       <c r="C53" s="4"/>
       <c r="D53">
         <v>3.23</v>
@@ -1826,7 +2023,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
-      <c r="B54" s="7"/>
+      <c r="B54" s="6"/>
       <c r="C54" s="4"/>
       <c r="D54">
         <v>3.24</v>
@@ -1837,7 +2034,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
-      <c r="B55" s="7"/>
+      <c r="B55" s="6"/>
       <c r="C55" s="4"/>
       <c r="D55">
         <v>3.25</v>
@@ -1848,7 +2045,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="7"/>
+      <c r="B56" s="6"/>
       <c r="C56" s="4"/>
       <c r="D56">
         <v>3.26</v>
@@ -1859,7 +2056,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
-      <c r="B57" s="7"/>
+      <c r="B57" s="6"/>
       <c r="C57" s="4"/>
       <c r="D57">
         <v>3.27</v>
@@ -1873,7 +2070,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
-      <c r="B58" s="7"/>
+      <c r="B58" s="6"/>
       <c r="C58" s="4"/>
       <c r="D58">
         <v>3.28</v>
@@ -1884,7 +2081,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
-      <c r="B59" s="7"/>
+      <c r="B59" s="6"/>
       <c r="C59" s="4"/>
       <c r="D59">
         <v>3.29</v>
@@ -1895,7 +2092,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
-      <c r="B60" s="7"/>
+      <c r="B60" s="6"/>
       <c r="C60" s="4"/>
       <c r="D60" s="1">
         <v>3.3</v>
@@ -1906,7 +2103,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
-      <c r="B61" s="7"/>
+      <c r="B61" s="6"/>
       <c r="C61" s="4"/>
       <c r="D61">
         <v>3.31</v>
@@ -1917,7 +2114,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
-      <c r="B62" s="7"/>
+      <c r="B62" s="6"/>
       <c r="C62" s="4"/>
       <c r="D62">
         <v>3.39</v>
@@ -1928,7 +2125,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
-      <c r="B63" s="7"/>
+      <c r="B63" s="6"/>
       <c r="C63" s="4"/>
       <c r="D63" s="1">
         <v>3.4</v>
@@ -1939,7 +2136,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
-      <c r="B64" s="7"/>
+      <c r="B64" s="6"/>
       <c r="C64" s="4"/>
       <c r="D64">
         <v>3.32</v>
@@ -1953,7 +2150,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
-      <c r="B65" s="7"/>
+      <c r="B65" s="6"/>
       <c r="C65" s="4"/>
       <c r="D65">
         <v>3.33</v>
@@ -1964,7 +2161,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
-      <c r="B66" s="7"/>
+      <c r="B66" s="6"/>
       <c r="C66" s="4"/>
       <c r="D66">
         <v>3.34</v>
@@ -1975,7 +2172,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
-      <c r="B67" s="7"/>
+      <c r="B67" s="6"/>
       <c r="C67" s="4"/>
       <c r="D67">
         <v>3.35</v>
@@ -1986,7 +2183,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
-      <c r="B68" s="7"/>
+      <c r="B68" s="6"/>
       <c r="C68" s="4"/>
       <c r="D68">
         <v>3.36</v>
@@ -1997,7 +2194,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
-      <c r="B69" s="7"/>
+      <c r="B69" s="6"/>
       <c r="C69" s="4"/>
       <c r="D69">
         <v>3.37</v>
@@ -2008,7 +2205,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
-      <c r="B70" s="7"/>
+      <c r="B70" s="6"/>
       <c r="C70" s="4"/>
       <c r="D70">
         <v>3.38</v>
@@ -2019,7 +2216,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
-      <c r="B71" s="7"/>
+      <c r="B71" s="6"/>
       <c r="C71" s="4" t="s">
         <v>81</v>
       </c>
@@ -2032,7 +2229,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
-      <c r="B72" s="7"/>
+      <c r="B72" s="6"/>
       <c r="C72" s="4"/>
       <c r="D72">
         <v>4.2</v>
@@ -2043,7 +2240,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
-      <c r="B73" s="7"/>
+      <c r="B73" s="6"/>
       <c r="C73" s="4"/>
       <c r="D73">
         <v>4.3</v>
@@ -2054,7 +2251,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
-      <c r="B74" s="7"/>
+      <c r="B74" s="6"/>
       <c r="C74" s="4"/>
       <c r="D74">
         <v>4.4000000000000004</v>
@@ -2065,7 +2262,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
-      <c r="B75" s="7"/>
+      <c r="B75" s="6"/>
       <c r="C75" s="4"/>
       <c r="D75">
         <v>4.5</v>
@@ -2076,7 +2273,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
-      <c r="B76" s="7"/>
+      <c r="B76" s="6"/>
       <c r="C76" s="4"/>
       <c r="D76">
         <v>4.5999999999999996</v>
@@ -2087,7 +2284,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
-      <c r="B77" s="7"/>
+      <c r="B77" s="6"/>
       <c r="C77" s="4"/>
       <c r="D77">
         <v>4.7</v>
@@ -2098,7 +2295,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
-      <c r="B78" s="7"/>
+      <c r="B78" s="6"/>
       <c r="C78" s="4"/>
       <c r="D78">
         <v>4.8</v>
@@ -2109,7 +2306,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
-      <c r="B79" s="7"/>
+      <c r="B79" s="6"/>
       <c r="C79" s="4"/>
       <c r="D79">
         <v>4.9000000000000004</v>
@@ -2120,7 +2317,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
-      <c r="B80" s="7"/>
+      <c r="B80" s="6"/>
       <c r="C80" s="4"/>
       <c r="D80" s="1">
         <v>4.0999999999999996</v>
@@ -2131,7 +2328,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
-      <c r="B81" s="7"/>
+      <c r="B81" s="6"/>
       <c r="C81" s="4"/>
       <c r="D81">
         <v>4.1100000000000003</v>
@@ -2142,7 +2339,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
-      <c r="B82" s="7"/>
+      <c r="B82" s="6"/>
       <c r="C82" s="4"/>
       <c r="D82">
         <v>4.12</v>
@@ -2153,7 +2350,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
-      <c r="B83" s="7"/>
+      <c r="B83" s="6"/>
       <c r="C83" s="4"/>
       <c r="D83">
         <v>4.13</v>
@@ -2164,7 +2361,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
-      <c r="B84" s="7"/>
+      <c r="B84" s="6"/>
       <c r="C84" s="4"/>
       <c r="D84">
         <v>4.1399999999999997</v>
@@ -2175,7 +2372,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
-      <c r="B85" s="7"/>
+      <c r="B85" s="6"/>
       <c r="C85" s="4"/>
       <c r="D85">
         <v>4.1500000000000004</v>
@@ -2186,7 +2383,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
-      <c r="B86" s="7"/>
+      <c r="B86" s="6"/>
       <c r="C86" s="4"/>
       <c r="D86">
         <v>4.16</v>
@@ -2197,7 +2394,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
-      <c r="B87" s="7"/>
+      <c r="B87" s="6"/>
       <c r="C87" s="4"/>
       <c r="D87">
         <v>4.17</v>
@@ -2208,7 +2405,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
-      <c r="B88" s="7"/>
+      <c r="B88" s="6"/>
       <c r="C88" s="4"/>
       <c r="D88">
         <v>4.2300000000000004</v>
@@ -2219,7 +2416,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
-      <c r="B89" s="7"/>
+      <c r="B89" s="6"/>
       <c r="C89" s="4"/>
       <c r="D89">
         <v>4.24</v>
@@ -2230,7 +2427,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
-      <c r="B90" s="7"/>
+      <c r="B90" s="6"/>
       <c r="C90" s="4"/>
       <c r="D90">
         <v>4.18</v>
@@ -2244,7 +2441,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
-      <c r="B91" s="7"/>
+      <c r="B91" s="6"/>
       <c r="C91" s="4"/>
       <c r="D91">
         <v>4.1900000000000004</v>
@@ -2255,7 +2452,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
-      <c r="B92" s="7"/>
+      <c r="B92" s="6"/>
       <c r="C92" s="4"/>
       <c r="D92" s="1">
         <v>4.2</v>
@@ -2266,7 +2463,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
-      <c r="B93" s="7"/>
+      <c r="B93" s="6"/>
       <c r="C93" s="4"/>
       <c r="D93">
         <v>4.21</v>
@@ -2277,7 +2474,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
-      <c r="B94" s="7"/>
+      <c r="B94" s="6"/>
       <c r="C94" s="4"/>
       <c r="D94">
         <v>4.22</v>
@@ -2287,8 +2484,8 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="7"/>
-      <c r="C95" s="6" t="s">
+      <c r="B95" s="6"/>
+      <c r="C95" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D95">
@@ -2299,8 +2496,8 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B96" s="7"/>
-      <c r="C96" s="6"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="5"/>
       <c r="D96">
         <v>5.2</v>
       </c>
@@ -2309,10 +2506,10 @@
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C97" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D97">
@@ -2323,8 +2520,8 @@
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B98" s="5"/>
-      <c r="C98" s="8"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="7"/>
       <c r="D98">
         <v>1.2</v>
       </c>
@@ -2333,7 +2530,7 @@
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B99" s="5"/>
+      <c r="B99" s="9"/>
       <c r="C99" s="4" t="s">
         <v>111</v>
       </c>
@@ -2345,7 +2542,7 @@
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="5"/>
+      <c r="B100" s="9"/>
       <c r="C100" s="4"/>
       <c r="D100">
         <v>2.2000000000000002</v>
@@ -2355,7 +2552,7 @@
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B101" s="5"/>
+      <c r="B101" s="9"/>
       <c r="C101" s="4"/>
       <c r="D101">
         <v>2.2999999999999998</v>
@@ -2365,7 +2562,7 @@
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="5"/>
+      <c r="B102" s="9"/>
       <c r="C102" s="4"/>
       <c r="D102">
         <v>2.4</v>
@@ -2375,7 +2572,7 @@
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B103" s="5"/>
+      <c r="B103" s="9"/>
       <c r="C103" s="4"/>
       <c r="D103">
         <v>2.5</v>
@@ -2385,7 +2582,7 @@
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="5"/>
+      <c r="B104" s="9"/>
       <c r="C104" s="4"/>
       <c r="D104">
         <v>2.6</v>
@@ -2395,7 +2592,7 @@
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B105" s="5"/>
+      <c r="B105" s="9"/>
       <c r="C105" s="4"/>
       <c r="D105">
         <v>2.7</v>
@@ -2405,7 +2602,7 @@
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B106" s="5"/>
+      <c r="B106" s="9"/>
       <c r="C106" s="4"/>
       <c r="D106">
         <v>2.8</v>
@@ -2415,7 +2612,7 @@
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B107" s="5"/>
+      <c r="B107" s="9"/>
       <c r="C107" s="4"/>
       <c r="D107">
         <v>2.9</v>
@@ -2425,7 +2622,7 @@
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B108" s="5"/>
+      <c r="B108" s="9"/>
       <c r="C108" s="4"/>
       <c r="D108" s="1">
         <v>2.1</v>
@@ -2435,7 +2632,7 @@
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B109" s="5"/>
+      <c r="B109" s="9"/>
       <c r="C109" s="4"/>
       <c r="D109">
         <v>2.11</v>
@@ -2445,7 +2642,7 @@
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="5"/>
+      <c r="B110" s="9"/>
       <c r="C110" s="4"/>
       <c r="D110">
         <v>2.12</v>
@@ -2455,7 +2652,7 @@
       </c>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B111" s="5"/>
+      <c r="B111" s="9"/>
       <c r="C111" s="4"/>
       <c r="D111">
         <v>2.13</v>
@@ -2465,7 +2662,7 @@
       </c>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B112" s="5"/>
+      <c r="B112" s="9"/>
       <c r="C112" s="4"/>
       <c r="D112">
         <v>2.14</v>
@@ -2475,7 +2672,7 @@
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B113" s="5"/>
+      <c r="B113" s="9"/>
       <c r="C113" s="4"/>
       <c r="D113">
         <v>2.15</v>
@@ -2485,7 +2682,7 @@
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B114" s="5"/>
+      <c r="B114" s="9"/>
       <c r="C114" s="4"/>
       <c r="D114">
         <v>2.16</v>
@@ -2495,7 +2692,7 @@
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B115" s="5"/>
+      <c r="B115" s="9"/>
       <c r="C115" s="4"/>
       <c r="D115">
         <v>2.17</v>
@@ -2505,7 +2702,7 @@
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B116" s="5"/>
+      <c r="B116" s="9"/>
       <c r="C116" s="4"/>
       <c r="D116">
         <v>2.1800000000000002</v>
@@ -2515,7 +2712,7 @@
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B117" s="5"/>
+      <c r="B117" s="9"/>
       <c r="C117" s="4"/>
       <c r="D117">
         <v>2.19</v>
@@ -2525,7 +2722,7 @@
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="5"/>
+      <c r="B118" s="9"/>
       <c r="C118" s="4"/>
       <c r="D118">
         <v>2.2000000000000002</v>
@@ -2535,7 +2732,7 @@
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B119" s="5"/>
+      <c r="B119" s="9"/>
       <c r="C119" s="4"/>
       <c r="D119">
         <v>2.21</v>
@@ -2545,7 +2742,7 @@
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B120" s="5"/>
+      <c r="B120" s="9"/>
       <c r="C120" s="4"/>
       <c r="D120">
         <v>2.23</v>
@@ -2555,7 +2752,7 @@
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B121" s="5"/>
+      <c r="B121" s="9"/>
       <c r="C121" s="4"/>
       <c r="D121">
         <v>2.2400000000000002</v>
@@ -2568,7 +2765,7 @@
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B122" s="5"/>
+      <c r="B122" s="9"/>
       <c r="C122" s="4"/>
       <c r="D122" s="1">
         <v>2.25</v>
@@ -2578,7 +2775,7 @@
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="5"/>
+      <c r="B123" s="9"/>
       <c r="C123" s="4"/>
       <c r="D123">
         <v>2.2599999999999998</v>
@@ -2588,7 +2785,7 @@
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B124" s="5"/>
+      <c r="B124" s="9"/>
       <c r="C124" s="4"/>
       <c r="D124" s="1">
         <v>2.2200000000000002</v>
@@ -2598,7 +2795,7 @@
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B125" s="5"/>
+      <c r="B125" s="9"/>
       <c r="C125" s="4"/>
       <c r="D125">
         <v>2.33</v>
@@ -2608,7 +2805,7 @@
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B126" s="5"/>
+      <c r="B126" s="9"/>
       <c r="C126" s="4"/>
       <c r="D126" s="1">
         <v>2.34</v>
@@ -2618,7 +2815,7 @@
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B127" s="5"/>
+      <c r="B127" s="9"/>
       <c r="C127" s="4"/>
       <c r="D127">
         <v>2.27</v>
@@ -2628,7 +2825,7 @@
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B128" s="5"/>
+      <c r="B128" s="9"/>
       <c r="C128" s="4"/>
       <c r="D128" s="1">
         <v>2.2799999999999998</v>
@@ -2638,7 +2835,7 @@
       </c>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B129" s="5"/>
+      <c r="B129" s="9"/>
       <c r="C129" s="4"/>
       <c r="D129">
         <v>2.29</v>
@@ -2648,7 +2845,7 @@
       </c>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B130" s="5"/>
+      <c r="B130" s="9"/>
       <c r="C130" s="4"/>
       <c r="D130" s="1">
         <v>2.2999999999999998</v>
@@ -2658,7 +2855,7 @@
       </c>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B131" s="5"/>
+      <c r="B131" s="9"/>
       <c r="C131" s="4"/>
       <c r="D131">
         <v>2.31</v>
@@ -2668,7 +2865,7 @@
       </c>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B132" s="5"/>
+      <c r="B132" s="9"/>
       <c r="C132" s="4"/>
       <c r="D132" s="1">
         <v>2.3199999999999998</v>
@@ -2678,7 +2875,7 @@
       </c>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B133" s="5"/>
+      <c r="B133" s="9"/>
       <c r="C133" s="3" t="s">
         <v>165</v>
       </c>
@@ -2690,7 +2887,7 @@
       </c>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B134" s="5"/>
+      <c r="B134" s="9"/>
       <c r="C134" s="3"/>
       <c r="D134" s="2">
         <v>3.2</v>
@@ -2700,7 +2897,7 @@
       </c>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="5"/>
+      <c r="B135" s="9"/>
       <c r="C135" s="3"/>
       <c r="D135" s="2">
         <v>3.3</v>
@@ -2710,7 +2907,7 @@
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B136" s="5"/>
+      <c r="B136" s="9"/>
       <c r="C136" s="3"/>
       <c r="D136" s="2">
         <v>3.4</v>
@@ -2720,7 +2917,7 @@
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="5"/>
+      <c r="B137" s="9"/>
       <c r="C137" s="3"/>
       <c r="D137" s="2">
         <v>3.5</v>
@@ -2730,7 +2927,7 @@
       </c>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B138" s="5"/>
+      <c r="B138" s="9"/>
       <c r="C138" s="3"/>
       <c r="D138" s="2">
         <v>3.6</v>
@@ -2740,7 +2937,7 @@
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B139" s="5"/>
+      <c r="B139" s="9"/>
       <c r="C139" s="3"/>
       <c r="D139" s="2">
         <v>3.7</v>
@@ -2750,7 +2947,7 @@
       </c>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B140" s="5"/>
+      <c r="B140" s="9"/>
       <c r="C140" s="3"/>
       <c r="D140" s="2">
         <v>3.8</v>
@@ -2760,7 +2957,7 @@
       </c>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B141" s="5"/>
+      <c r="B141" s="9"/>
       <c r="C141" s="3"/>
       <c r="D141" s="2">
         <v>3.9</v>
@@ -2770,7 +2967,7 @@
       </c>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B142" s="5"/>
+      <c r="B142" s="9"/>
       <c r="C142" s="3"/>
       <c r="D142" s="1">
         <v>3.1</v>
@@ -2780,7 +2977,7 @@
       </c>
     </row>
     <row r="143" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B143" s="5"/>
+      <c r="B143" s="9"/>
       <c r="C143" s="3"/>
       <c r="D143" s="2">
         <v>3.11</v>
@@ -2790,7 +2987,7 @@
       </c>
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B144" s="5"/>
+      <c r="B144" s="9"/>
       <c r="C144" s="3"/>
       <c r="D144" s="2">
         <v>3.12</v>
@@ -2800,7 +2997,7 @@
       </c>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B145" s="5"/>
+      <c r="B145" s="9"/>
       <c r="C145" s="3"/>
       <c r="D145" s="2">
         <v>3.13</v>
@@ -2810,7 +3007,7 @@
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B146" s="5"/>
+      <c r="B146" s="9"/>
       <c r="C146" s="3"/>
       <c r="D146" s="2">
         <v>3.14</v>
@@ -2820,7 +3017,7 @@
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B147" s="5"/>
+      <c r="B147" s="9"/>
       <c r="C147" s="3"/>
       <c r="D147" s="2">
         <v>3.15</v>
@@ -2830,7 +3027,7 @@
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B148" s="5"/>
+      <c r="B148" s="9"/>
       <c r="C148" s="3"/>
       <c r="D148" s="2">
         <v>3.16</v>
@@ -2840,7 +3037,7 @@
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B149" s="5"/>
+      <c r="B149" s="9"/>
       <c r="C149" s="3"/>
       <c r="D149" s="2">
         <v>3.17</v>
@@ -2850,7 +3047,7 @@
       </c>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B150" s="5"/>
+      <c r="B150" s="9"/>
       <c r="C150" s="3"/>
       <c r="D150" s="2">
         <v>3.18</v>
@@ -2860,7 +3057,7 @@
       </c>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B151" s="5"/>
+      <c r="B151" s="9"/>
       <c r="C151" s="3"/>
       <c r="D151" s="2">
         <v>3.19</v>
@@ -2870,7 +3067,7 @@
       </c>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B152" s="5"/>
+      <c r="B152" s="9"/>
       <c r="C152" s="3"/>
       <c r="D152" s="1">
         <v>3.2</v>
@@ -2880,7 +3077,7 @@
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B153" s="5"/>
+      <c r="B153" s="9"/>
       <c r="C153" s="3"/>
       <c r="D153" s="2">
         <v>3.21</v>
@@ -2890,7 +3087,7 @@
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B154" s="5"/>
+      <c r="B154" s="9"/>
       <c r="C154" s="3"/>
       <c r="D154" s="2">
         <v>3.22</v>
@@ -2900,7 +3097,7 @@
       </c>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B155" s="5"/>
+      <c r="B155" s="9"/>
       <c r="C155" s="3"/>
       <c r="D155" s="2">
         <v>3.23</v>
@@ -2910,7 +3107,7 @@
       </c>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B156" s="5"/>
+      <c r="B156" s="9"/>
       <c r="C156" s="3"/>
       <c r="D156" s="2">
         <v>3.24</v>
@@ -2920,7 +3117,7 @@
       </c>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B157" s="5"/>
+      <c r="B157" s="9"/>
       <c r="C157" s="3"/>
       <c r="D157" s="2">
         <v>3.25</v>
@@ -2930,7 +3127,7 @@
       </c>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B158" s="5"/>
+      <c r="B158" s="9"/>
       <c r="C158" s="3"/>
       <c r="D158" s="2">
         <v>3.26</v>
@@ -2940,7 +3137,7 @@
       </c>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B159" s="5"/>
+      <c r="B159" s="9"/>
       <c r="C159" s="3"/>
       <c r="D159" s="2">
         <v>3.27</v>
@@ -2950,7 +3147,7 @@
       </c>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B160" s="5"/>
+      <c r="B160" s="9"/>
       <c r="C160" s="3"/>
       <c r="D160" s="2">
         <v>3.28</v>
@@ -2960,7 +3157,7 @@
       </c>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B161" s="5"/>
+      <c r="B161" s="9"/>
       <c r="C161" s="3"/>
       <c r="D161" s="2">
         <v>3.29</v>
@@ -2970,7 +3167,7 @@
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B162" s="5"/>
+      <c r="B162" s="9"/>
       <c r="C162" s="3"/>
       <c r="D162" s="1">
         <v>3.3</v>
@@ -2980,7 +3177,7 @@
       </c>
     </row>
     <row r="163" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B163" s="5"/>
+      <c r="B163" s="9"/>
       <c r="C163" s="3"/>
       <c r="D163" s="2">
         <v>3.31</v>
@@ -2990,7 +3187,7 @@
       </c>
     </row>
     <row r="164" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B164" s="5"/>
+      <c r="B164" s="9"/>
       <c r="C164" s="3"/>
       <c r="D164" s="2">
         <v>3.32</v>
@@ -3000,7 +3197,7 @@
       </c>
     </row>
     <row r="165" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B165" s="5"/>
+      <c r="B165" s="9"/>
       <c r="C165" s="3"/>
       <c r="D165" s="2">
         <v>3.33</v>
@@ -3010,7 +3207,7 @@
       </c>
     </row>
     <row r="166" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B166" s="5"/>
+      <c r="B166" s="9"/>
       <c r="C166" s="3"/>
       <c r="D166" s="2">
         <v>3.34</v>
@@ -3020,7 +3217,7 @@
       </c>
     </row>
     <row r="167" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B167" s="5"/>
+      <c r="B167" s="9"/>
       <c r="C167" s="3"/>
       <c r="D167" s="2">
         <v>3.35</v>
@@ -3030,7 +3227,7 @@
       </c>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B168" s="5"/>
+      <c r="B168" s="9"/>
       <c r="C168" s="3"/>
       <c r="D168" s="2">
         <v>3.42</v>
@@ -3040,7 +3237,7 @@
       </c>
     </row>
     <row r="169" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B169" s="5"/>
+      <c r="B169" s="9"/>
       <c r="C169" s="3"/>
       <c r="D169" s="2">
         <v>3.43</v>
@@ -3050,7 +3247,7 @@
       </c>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B170" s="5"/>
+      <c r="B170" s="9"/>
       <c r="C170" s="3"/>
       <c r="D170" s="2">
         <v>3.36</v>
@@ -3060,7 +3257,7 @@
       </c>
     </row>
     <row r="171" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B171" s="5"/>
+      <c r="B171" s="9"/>
       <c r="C171" s="3"/>
       <c r="D171" s="2">
         <v>3.37</v>
@@ -3070,7 +3267,7 @@
       </c>
     </row>
     <row r="172" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B172" s="5"/>
+      <c r="B172" s="9"/>
       <c r="D172" s="2">
         <v>3.38</v>
       </c>
@@ -3079,7 +3276,7 @@
       </c>
     </row>
     <row r="173" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B173" s="5"/>
+      <c r="B173" s="9"/>
       <c r="D173" s="2">
         <v>3.39</v>
       </c>
@@ -3088,7 +3285,7 @@
       </c>
     </row>
     <row r="174" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B174" s="5"/>
+      <c r="B174" s="9"/>
       <c r="D174" s="1">
         <v>3.4</v>
       </c>
@@ -3097,9 +3294,7 @@
       </c>
     </row>
     <row r="175" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
-        <v>168</v>
-      </c>
+      <c r="B175" s="9"/>
       <c r="D175">
         <v>3.41</v>
       </c>
@@ -3108,6 +3303,7 @@
       </c>
     </row>
     <row r="176" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B176" s="9"/>
       <c r="C176" s="4" t="s">
         <v>166</v>
       </c>
@@ -3118,7 +3314,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="177" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B177" s="9"/>
       <c r="C177" s="4"/>
       <c r="D177">
         <v>4.2</v>
@@ -3127,7 +3324,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="178" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B178" s="9"/>
       <c r="C178" s="4"/>
       <c r="D178">
         <v>4.3</v>
@@ -3136,7 +3334,10 @@
         <v>167</v>
       </c>
     </row>
-    <row r="179" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B179" s="8" t="s">
+        <v>168</v>
+      </c>
       <c r="C179" s="4" t="s">
         <v>37</v>
       </c>
@@ -3147,7 +3348,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B180" s="8"/>
       <c r="C180" s="4"/>
       <c r="D180">
         <v>1.2</v>
@@ -3156,7 +3358,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B181" s="8"/>
       <c r="C181" s="3" t="s">
         <v>198</v>
       </c>
@@ -3167,7 +3370,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B182" s="8"/>
       <c r="C182" s="3"/>
       <c r="D182">
         <v>2.2000000000000002</v>
@@ -3176,7 +3380,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B183" s="8"/>
       <c r="C183" s="3"/>
       <c r="D183">
         <v>2.2999999999999998</v>
@@ -3185,7 +3390,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B184" s="8"/>
       <c r="C184" s="3"/>
       <c r="D184">
         <v>2.4</v>
@@ -3194,7 +3400,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="185" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B185" s="8"/>
       <c r="C185" s="3"/>
       <c r="D185">
         <v>2.5</v>
@@ -3203,7 +3410,8 @@
         <v>170</v>
       </c>
     </row>
-    <row r="186" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B186" s="8"/>
       <c r="C186" s="3"/>
       <c r="D186">
         <v>2.6</v>
@@ -3212,7 +3420,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="187" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B187" s="8"/>
       <c r="C187" s="3"/>
       <c r="D187">
         <v>2.7</v>
@@ -3221,7 +3430,8 @@
         <v>172</v>
       </c>
     </row>
-    <row r="188" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B188" s="8"/>
       <c r="C188" s="3"/>
       <c r="D188">
         <v>2.8</v>
@@ -3230,7 +3440,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="189" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B189" s="8"/>
       <c r="C189" s="3"/>
       <c r="D189">
         <v>2.9</v>
@@ -3239,7 +3450,8 @@
         <v>174</v>
       </c>
     </row>
-    <row r="190" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B190" s="8"/>
       <c r="C190" s="3"/>
       <c r="D190" s="1">
         <v>2.1</v>
@@ -3248,7 +3460,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="191" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B191" s="8"/>
       <c r="C191" s="3"/>
       <c r="D191">
         <v>2.11</v>
@@ -3257,7 +3470,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="192" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B192" s="8"/>
       <c r="C192" s="3"/>
       <c r="D192">
         <v>2.12</v>
@@ -3266,7 +3480,8 @@
         <v>185</v>
       </c>
     </row>
-    <row r="193" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B193" s="8"/>
       <c r="C193" s="3"/>
       <c r="D193">
         <v>2.13</v>
@@ -3275,7 +3490,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="194" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B194" s="8"/>
       <c r="C194" s="3"/>
       <c r="D194">
         <v>2.14</v>
@@ -3284,7 +3500,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="195" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B195" s="8"/>
       <c r="C195" s="3"/>
       <c r="D195">
         <v>2.15</v>
@@ -3293,7 +3510,8 @@
         <v>177</v>
       </c>
     </row>
-    <row r="196" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B196" s="8"/>
       <c r="C196" s="3"/>
       <c r="D196">
         <v>2.16</v>
@@ -3302,7 +3520,8 @@
         <v>178</v>
       </c>
     </row>
-    <row r="197" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B197" s="8"/>
       <c r="C197" s="3"/>
       <c r="D197">
         <v>2.17</v>
@@ -3311,7 +3530,8 @@
         <v>179</v>
       </c>
     </row>
-    <row r="198" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B198" s="8"/>
       <c r="C198" s="3"/>
       <c r="D198">
         <v>2.1800000000000002</v>
@@ -3320,7 +3540,8 @@
         <v>181</v>
       </c>
     </row>
-    <row r="199" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B199" s="8"/>
       <c r="C199" s="3"/>
       <c r="D199">
         <v>2.19</v>
@@ -3329,7 +3550,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="200" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B200" s="8"/>
       <c r="C200" s="3"/>
       <c r="D200" s="1">
         <v>2.2000000000000002</v>
@@ -3338,7 +3560,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="201" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B201" s="8"/>
       <c r="C201" s="3"/>
       <c r="D201">
         <v>2.21</v>
@@ -3347,7 +3570,8 @@
         <v>184</v>
       </c>
     </row>
-    <row r="202" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B202" s="8"/>
       <c r="C202" s="3"/>
       <c r="D202">
         <v>2.2200000000000002</v>
@@ -3356,7 +3580,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="203" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B203" s="8"/>
       <c r="C203" s="3"/>
       <c r="D203">
         <v>2.23</v>
@@ -3365,7 +3590,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="204" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B204" s="8"/>
       <c r="C204" s="3"/>
       <c r="D204">
         <v>2.2400000000000002</v>
@@ -3374,7 +3600,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="205" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B205" s="8"/>
       <c r="C205" s="3"/>
       <c r="D205">
         <v>2.25</v>
@@ -3383,7 +3610,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="206" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B206" s="8"/>
       <c r="C206" s="3"/>
       <c r="D206">
         <v>2.2599999999999998</v>
@@ -3392,7 +3620,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="207" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B207" s="8"/>
       <c r="C207" s="3"/>
       <c r="D207">
         <v>2.27</v>
@@ -3401,7 +3630,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B208" s="8"/>
       <c r="C208" s="3"/>
       <c r="D208">
         <v>2.2799999999999998</v>
@@ -3410,7 +3640,8 @@
         <v>190</v>
       </c>
     </row>
-    <row r="209" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B209" s="8"/>
       <c r="C209" s="3"/>
       <c r="D209">
         <v>2.29</v>
@@ -3419,7 +3650,8 @@
         <v>191</v>
       </c>
     </row>
-    <row r="210" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B210" s="8"/>
       <c r="C210" s="3"/>
       <c r="D210" s="1">
         <v>2.2999999999999998</v>
@@ -3428,7 +3660,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="211" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B211" s="8"/>
       <c r="C211" s="3"/>
       <c r="D211">
         <v>2.31</v>
@@ -3437,7 +3670,8 @@
         <v>193</v>
       </c>
     </row>
-    <row r="212" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B212" s="8"/>
       <c r="C212" s="3"/>
       <c r="D212">
         <v>2.3199999999999998</v>
@@ -3446,7 +3680,8 @@
         <v>194</v>
       </c>
     </row>
-    <row r="213" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B213" s="8"/>
       <c r="C213" s="3"/>
       <c r="D213">
         <v>2.33</v>
@@ -3455,7 +3690,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="214" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B214" s="8"/>
       <c r="C214" s="3"/>
       <c r="D214">
         <v>2.34</v>
@@ -3464,7 +3700,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="215" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B215" s="8"/>
       <c r="C215" s="3"/>
       <c r="D215">
         <v>2.35</v>
@@ -3473,7 +3710,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="216" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B216" s="8"/>
       <c r="C216" s="3"/>
       <c r="D216">
         <v>2.36</v>
@@ -3482,7 +3720,8 @@
         <v>195</v>
       </c>
     </row>
-    <row r="217" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B217" s="8"/>
       <c r="C217" s="3"/>
       <c r="D217">
         <v>2.37</v>
@@ -3491,7 +3730,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="218" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B218" s="8"/>
       <c r="C218" s="3"/>
       <c r="D218">
         <v>2.38</v>
@@ -3500,7 +3740,8 @@
         <v>189</v>
       </c>
     </row>
-    <row r="219" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B219" s="8"/>
       <c r="C219" s="3"/>
       <c r="D219">
         <v>2.39</v>
@@ -3509,7 +3750,8 @@
         <v>197</v>
       </c>
     </row>
-    <row r="220" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B220" s="8"/>
       <c r="C220" s="3"/>
       <c r="D220" s="1">
         <v>2.4</v>
@@ -3518,7 +3760,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="221" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B221" s="8"/>
       <c r="C221" s="3"/>
       <c r="D221">
         <v>2.41</v>
@@ -3527,7 +3770,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="222" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B222" s="8"/>
       <c r="C222" s="3"/>
       <c r="D222">
         <v>2.42</v>
@@ -3536,7 +3780,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="223" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B223" s="8"/>
       <c r="C223" t="s">
         <v>199</v>
       </c>
@@ -3547,7 +3792,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="224" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B224" s="8"/>
       <c r="D224">
         <v>3.2</v>
       </c>
@@ -3555,7 +3801,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="225" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B225" s="8"/>
       <c r="D225">
         <v>3.3</v>
       </c>
@@ -3563,7 +3810,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="226" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B226" s="8"/>
       <c r="D226">
         <v>3.4</v>
       </c>
@@ -3571,7 +3819,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="227" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B227" s="8"/>
       <c r="D227">
         <v>3.5</v>
       </c>
@@ -3579,7 +3828,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="228" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B228" s="8"/>
       <c r="D228">
         <v>3.6</v>
       </c>
@@ -3587,7 +3837,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="229" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B229" s="8"/>
       <c r="D229">
         <v>3.7</v>
       </c>
@@ -3595,7 +3846,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="230" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B230" s="8"/>
       <c r="D230">
         <v>3.8</v>
       </c>
@@ -3603,7 +3855,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="231" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B231" s="8"/>
       <c r="D231">
         <v>3.9</v>
       </c>
@@ -3611,7 +3864,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="232" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B232" s="8"/>
       <c r="D232" s="1">
         <v>3.1</v>
       </c>
@@ -3619,7 +3873,8 @@
         <v>206</v>
       </c>
     </row>
-    <row r="233" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B233" s="8"/>
       <c r="D233">
         <v>3.11</v>
       </c>
@@ -3627,7 +3882,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="234" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B234" s="8"/>
       <c r="D234">
         <v>3.12</v>
       </c>
@@ -3635,7 +3891,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="235" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B235" s="8"/>
       <c r="D235">
         <v>3.13</v>
       </c>
@@ -3643,7 +3900,8 @@
         <v>209</v>
       </c>
     </row>
-    <row r="236" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B236" s="8"/>
       <c r="D236">
         <v>3.14</v>
       </c>
@@ -3651,7 +3909,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="237" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B237" s="8"/>
       <c r="D237">
         <v>3.15</v>
       </c>
@@ -3659,7 +3918,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="238" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B238" s="8"/>
       <c r="D238">
         <v>3.16</v>
       </c>
@@ -3667,7 +3927,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="239" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B239" s="8"/>
       <c r="D239">
         <v>3.17</v>
       </c>
@@ -3675,7 +3936,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="240" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B240" s="8"/>
       <c r="D240">
         <v>3.18</v>
       </c>
@@ -3683,7 +3945,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="241" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B241" s="8"/>
       <c r="D241">
         <v>3.19</v>
       </c>
@@ -3691,7 +3954,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="242" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B242" s="8"/>
       <c r="D242" s="1">
         <v>3.2</v>
       </c>
@@ -3699,7 +3963,8 @@
         <v>213</v>
       </c>
     </row>
-    <row r="243" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B243" s="8"/>
       <c r="D243">
         <v>3.21</v>
       </c>
@@ -3707,7 +3972,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="244" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B244" s="8"/>
       <c r="D244">
         <v>3.28</v>
       </c>
@@ -3715,7 +3981,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="245" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B245" s="8"/>
       <c r="D245" s="1">
         <v>3.29</v>
       </c>
@@ -3723,7 +3990,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="246" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B246" s="8"/>
       <c r="D246">
         <v>3.22</v>
       </c>
@@ -3731,7 +3999,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="247" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B247" s="8"/>
       <c r="D247">
         <v>3.23</v>
       </c>
@@ -3739,7 +4008,8 @@
         <v>216</v>
       </c>
     </row>
-    <row r="248" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B248" s="8"/>
       <c r="D248">
         <v>3.24</v>
       </c>
@@ -3747,7 +4017,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="249" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B249" s="8"/>
       <c r="D249">
         <v>3.25</v>
       </c>
@@ -3755,7 +4026,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="250" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B250" s="8"/>
       <c r="D250">
         <v>3.26</v>
       </c>
@@ -3763,7 +4035,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="251" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B251" s="8"/>
       <c r="D251">
         <v>3.27</v>
       </c>
@@ -3771,7 +4044,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="252" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B252" s="8"/>
       <c r="C252" t="s">
         <v>217</v>
       </c>
@@ -3782,7 +4056,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="253" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B253" s="8"/>
       <c r="D253">
         <v>4.2</v>
       </c>
@@ -3790,7 +4065,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="254" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B254" s="8"/>
       <c r="D254">
         <v>4.3</v>
       </c>
@@ -3799,9 +4075,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="C179:C180"/>
-    <mergeCell ref="B97:B174"/>
     <mergeCell ref="C31:C70"/>
     <mergeCell ref="C71:C94"/>
     <mergeCell ref="A2:A94"/>
@@ -3812,6 +4087,8 @@
     <mergeCell ref="C97:C98"/>
     <mergeCell ref="C99:C132"/>
     <mergeCell ref="C176:C178"/>
+    <mergeCell ref="B179:B254"/>
+    <mergeCell ref="B97:B178"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3822,8 +4099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0CD2C6-46F0-4D9F-A783-CCE82B5FAC3A}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4397,4 +4674,885 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02102C7E-FB95-44F1-801E-818E96124A40}">
+  <dimension ref="A1:E93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="7"/>
+      <c r="C3">
+        <v>1.2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4">
+        <v>2.1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7">
+        <v>2.4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8">
+        <v>2.5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9">
+        <v>2.6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10">
+        <v>2.7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11">
+        <v>2.8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12">
+        <v>2.9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14">
+        <v>2.11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15">
+        <v>2.12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16">
+        <v>2.13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17">
+        <v>2.14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18">
+        <v>2.15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19">
+        <v>2.16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20">
+        <v>2.17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="D21" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22">
+        <v>2.19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23">
+        <v>2.21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25">
+        <v>2.23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="D26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27">
+        <v>2.25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="D28" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31">
+        <v>2.33</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32">
+        <v>2.27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="D33" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34">
+        <v>2.29</v>
+      </c>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36">
+        <v>2.31</v>
+      </c>
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C37">
+        <v>3.1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38">
+        <v>3.2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39">
+        <v>3.3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40">
+        <v>3.4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41">
+        <v>3.5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42">
+        <v>3.6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43">
+        <v>3.7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44">
+        <v>3.8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45">
+        <v>3.9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47">
+        <v>3.11</v>
+      </c>
+      <c r="D47" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48">
+        <v>3.12</v>
+      </c>
+      <c r="D48" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49">
+        <v>3.13</v>
+      </c>
+      <c r="D49" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50">
+        <v>3.14</v>
+      </c>
+      <c r="D50" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="4"/>
+      <c r="C51">
+        <v>3.15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52">
+        <v>3.16</v>
+      </c>
+      <c r="D52" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53">
+        <v>3.17</v>
+      </c>
+      <c r="D53" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4"/>
+      <c r="C54">
+        <v>3.18</v>
+      </c>
+      <c r="D54" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="4"/>
+      <c r="C55">
+        <v>3.19</v>
+      </c>
+      <c r="D55" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="4"/>
+      <c r="C57">
+        <v>3.21</v>
+      </c>
+      <c r="D57" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="4"/>
+      <c r="C58">
+        <v>3.22</v>
+      </c>
+      <c r="D58" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="C59">
+        <v>3.23</v>
+      </c>
+      <c r="D59" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="4"/>
+      <c r="C60">
+        <v>3.24</v>
+      </c>
+      <c r="D60" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="4"/>
+      <c r="C61">
+        <v>3.25</v>
+      </c>
+      <c r="D61" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62">
+        <v>3.26</v>
+      </c>
+      <c r="D62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="C63">
+        <v>3.27</v>
+      </c>
+      <c r="D63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64">
+        <v>3.28</v>
+      </c>
+      <c r="D64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65">
+        <v>3.29</v>
+      </c>
+      <c r="D65" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4"/>
+      <c r="C66">
+        <v>3.3</v>
+      </c>
+      <c r="D66" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4"/>
+      <c r="C67">
+        <v>3.31</v>
+      </c>
+      <c r="D67" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4"/>
+      <c r="C68">
+        <v>3.32</v>
+      </c>
+      <c r="D68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69">
+        <v>3.37</v>
+      </c>
+      <c r="D69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="C70">
+        <v>3.38</v>
+      </c>
+      <c r="D70" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="C71">
+        <v>3.33</v>
+      </c>
+      <c r="D71" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="4"/>
+      <c r="C72">
+        <v>3.34</v>
+      </c>
+      <c r="D72" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="4"/>
+      <c r="C73">
+        <v>3.35</v>
+      </c>
+      <c r="D73" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4"/>
+      <c r="C74">
+        <v>3.36</v>
+      </c>
+      <c r="D74" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+      <c r="C75">
+        <v>3.37</v>
+      </c>
+      <c r="D75" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C76">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D76" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="C77">
+        <v>4.2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="C78">
+        <v>4.3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>309</v>
+      </c>
+      <c r="B79" t="s">
+        <v>37</v>
+      </c>
+      <c r="C79">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D79" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>1.2</v>
+      </c>
+      <c r="D80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>111</v>
+      </c>
+      <c r="C81">
+        <v>2.1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>2.4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>2.5</v>
+      </c>
+      <c r="D85" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>2.6</v>
+      </c>
+      <c r="D86" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>2.7</v>
+      </c>
+      <c r="D87" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>2.8</v>
+      </c>
+      <c r="D88" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>2.9</v>
+      </c>
+      <c r="D89" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C90" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>2.11</v>
+      </c>
+      <c r="D91" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>2.12</v>
+      </c>
+      <c r="D92" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>2.13</v>
+      </c>
+      <c r="D93" t="s">
+        <v>319</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B36"/>
+    <mergeCell ref="B37:B75"/>
+    <mergeCell ref="B76:B78"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>